<commit_message>
Finished new absolute reference tutorial
</commit_message>
<xml_diff>
--- a/ch4-spreadsheets/res/tutorial_references.xlsx
+++ b/ch4-spreadsheets/res/tutorial_references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Payroll Report</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -69,9 +72,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +89,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -124,22 +144,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -443,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -620,12 +646,500 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774AE5C0-7DB5-4AC9-ACA1-67FA8D392641}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>B$1*$A2</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ref="C2:K11" si="0">C$1*$A2</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B11" si="1">B$1*$A3</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>